<commit_message>
Type3 ready? fixing details
</commit_message>
<xml_diff>
--- a/files/reservorio_empuje_agua.xlsx
+++ b/files/reservorio_empuje_agua.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\Desktop\py\ayllin\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1552AC08-70B2-43C9-9078-B821356624AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B6E135-327C-41B9-85B2-E4881C4D5FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9075" yWindow="3480" windowWidth="14415" windowHeight="11550" xr2:uid="{44499CD8-C7FF-4958-889A-4A80EC9AE5DF}"/>
+    <workbookView xWindow="0" yWindow="3930" windowWidth="14415" windowHeight="11550" xr2:uid="{44499CD8-C7FF-4958-889A-4A80EC9AE5DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
     <t>Yacimiento</t>
   </si>
   <si>
-    <t>Acuífero</t>
+    <t>Acuifero</t>
   </si>
 </sst>
 </file>
@@ -50,7 +50,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
-    <numFmt numFmtId="169" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -84,7 +84,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,7 +402,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>